<commit_message>
updated CanbusOff signal matrix and sharing the changes with Hanumana Created Arxml for the CanBusOffSWC
</commit_message>
<xml_diff>
--- a/R0/02_SignalMatrix/CanBusOff/CanBusOff_SignalMatrix_V1_R0.xlsx
+++ b/R0/02_SignalMatrix/CanBusOff/CanBusOff_SignalMatrix_V1_R0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veoneer-my.sharepoint.com/personal/kasi_subrahmanyam_veoneer_com/Documents/Documents/HKMC-Documents/CAN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R0\02_SignalMatrix\CanBusOff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{771B29DD-7427-4C9C-9E7F-49747FD6E8FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{341FC38F-B4D1-4C40-AA64-9B984D559832}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E125839-809E-434B-AE31-E417D42DE756}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="34500" yWindow="405" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>Change Log</t>
   </si>
@@ -130,9 +130,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -186,15 +183,6 @@
     <t xml:space="preserve"> Updated based on review comments</t>
   </si>
   <si>
-    <t>CanBusOff_Begin(networkHandle)</t>
-  </si>
-  <si>
-    <t>CanBusOff_End(networkHandle)</t>
-  </si>
-  <si>
-    <t>CanSM_BusOffIndicated(networkHandle)</t>
-  </si>
-  <si>
     <t>CanBusOffStatus</t>
   </si>
   <si>
@@ -234,24 +222,44 @@
     <t>Gives the Canbusoff status of the channel
 Bit0: CH1 CanBusOff (0-Normal, 1- Can Bus Off)
 Bit1: CH2 CanBusOff (0-Normal, 1- Can Bus Off)</t>
+  </si>
+  <si>
+    <t>networkHandle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Can_BusOffIndicated(networkHandle)/CanBusOff</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanBusOff_Begin(networkHandle)/CanBusOff</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanBusOff_End(networkHandle)/CanBusOff</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanBusOffStatus/CanBusOffStatus</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -262,7 +270,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -271,7 +279,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -279,20 +287,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -300,7 +308,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -308,7 +316,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -316,14 +324,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -407,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -685,6 +693,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -704,7 +723,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,6 +869,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1280,16 +1302,16 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="72.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="72.625" customWidth="1"/>
+    <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" customHeight="1">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1322,7 +1344,7 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
-    <row r="2" spans="1:31" ht="15" thickBot="1">
+    <row r="2" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1355,7 +1377,7 @@
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="45" t="s">
         <v>0</v>
@@ -1390,7 +1412,7 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
     </row>
-    <row r="4" spans="1:31" ht="15" thickBot="1">
+    <row r="4" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
         <v>1</v>
@@ -1431,7 +1453,7 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
     </row>
-    <row r="5" spans="1:31" ht="15" thickTop="1">
+    <row r="5" spans="1:31" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="10">
         <v>1</v>
@@ -1440,10 +1462,10 @@
         <v>43986</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="4"/>
@@ -1472,7 +1494,7 @@
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="15">
         <v>2</v>
@@ -1481,10 +1503,10 @@
         <v>43986</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="4"/>
@@ -1513,7 +1535,7 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="10">
         <v>3</v>
@@ -1522,10 +1544,10 @@
         <v>44047</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="4"/>
@@ -1554,7 +1576,7 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="15"/>
       <c r="C8" s="27"/>
@@ -1587,7 +1609,7 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -1620,7 +1642,7 @@
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -1653,7 +1675,7 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="10"/>
       <c r="C11" s="12"/>
@@ -1686,7 +1708,7 @@
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -1719,7 +1741,7 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="10"/>
       <c r="C13" s="12"/>
@@ -1752,7 +1774,7 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -1785,7 +1807,7 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="10"/>
       <c r="C15" s="12"/>
@@ -1818,7 +1840,7 @@
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
     </row>
-    <row r="16" spans="1:31" ht="15" thickBot="1">
+    <row r="16" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="19"/>
       <c r="C16" s="20"/>
@@ -1851,7 +1873,7 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1884,7 +1906,7 @@
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1917,7 +1939,7 @@
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1950,7 +1972,7 @@
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1983,7 +2005,7 @@
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2016,7 +2038,7 @@
       <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2049,7 +2071,7 @@
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2082,7 +2104,7 @@
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2115,7 +2137,7 @@
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2148,7 +2170,7 @@
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2181,7 +2203,7 @@
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2214,7 +2236,7 @@
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2247,7 +2269,7 @@
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2280,7 +2302,7 @@
       <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2313,7 +2335,7 @@
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2346,7 +2368,7 @@
       <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2379,7 +2401,7 @@
       <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2412,7 +2434,7 @@
       <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2445,7 +2467,7 @@
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2478,7 +2500,7 @@
       <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2511,7 +2533,7 @@
       <c r="AD36" s="4"/>
       <c r="AE36" s="4"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2544,7 +2566,7 @@
       <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2577,7 +2599,7 @@
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2610,7 +2632,7 @@
       <c r="AD39" s="4"/>
       <c r="AE39" s="4"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2643,7 +2665,7 @@
       <c r="AD40" s="4"/>
       <c r="AE40" s="4"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2676,7 +2698,7 @@
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2709,7 +2731,7 @@
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2742,7 +2764,7 @@
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2775,7 +2797,7 @@
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2808,7 +2830,7 @@
       <c r="AD45" s="4"/>
       <c r="AE45" s="4"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2841,7 +2863,7 @@
       <c r="AD46" s="4"/>
       <c r="AE46" s="4"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2874,7 +2896,7 @@
       <c r="AD47" s="4"/>
       <c r="AE47" s="4"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2907,7 +2929,7 @@
       <c r="AD48" s="4"/>
       <c r="AE48" s="4"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2940,7 +2962,7 @@
       <c r="AD49" s="4"/>
       <c r="AE49" s="4"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2973,7 +2995,7 @@
       <c r="AD50" s="4"/>
       <c r="AE50" s="4"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3024,35 +3046,35 @@
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="17.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="30.33203125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" style="30" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="17.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="30.375" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="30" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="31" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6.625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.44140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.88671875" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" style="33" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" customWidth="1"/>
-    <col min="19" max="19" width="14.44140625" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" customWidth="1"/>
-    <col min="21" max="21" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.875" customWidth="1"/>
+    <col min="17" max="17" width="23.375" style="33" customWidth="1"/>
+    <col min="18" max="18" width="21.5" customWidth="1"/>
+    <col min="19" max="19" width="14.5" customWidth="1"/>
+    <col min="20" max="20" width="15.625" customWidth="1"/>
+    <col min="21" max="21" width="92.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="57.6">
+    <row r="1" spans="1:21" ht="66" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
@@ -3081,19 +3103,19 @@
         <v>5</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="39" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="R1" s="29" t="s">
         <v>10</v>
       </c>
       <c r="S1" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>11</v>
@@ -3102,116 +3124,117 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="43.2">
+    <row r="2" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="N2" s="36">
         <v>1</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="36" t="s">
-        <v>42</v>
-      </c>
       <c r="R2" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="38" t="s">
         <v>19</v>
-      </c>
-      <c r="S2" s="38" t="s">
-        <v>20</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="U2" s="28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="43.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="M3" s="52"/>
       <c r="N3" s="36">
         <v>2</v>
       </c>
       <c r="O3" s="37" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="36" t="s">
-        <v>42</v>
-      </c>
       <c r="R3" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="38" t="s">
         <v>19</v>
-      </c>
-      <c r="S3" s="38" t="s">
-        <v>20</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="U3" s="28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="43.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="N4" s="36">
         <v>3</v>
       </c>
       <c r="O4" s="37" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="36" t="s">
-        <v>42</v>
-      </c>
       <c r="R4" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="38" t="s">
         <v>19</v>
-      </c>
-      <c r="S4" s="38" t="s">
-        <v>20</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="U4" s="28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="43.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="49.5" x14ac:dyDescent="0.3">
       <c r="N5" s="36">
         <v>4</v>
       </c>
       <c r="O5" s="37" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="P5" s="44" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="36"/>
       <c r="R5" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S5" s="38" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U5" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="O6"/>
       <c r="Q6"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="O8"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="O9"/>
     </row>
   </sheetData>
@@ -3247,30 +3270,30 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
-    <col min="7" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" customWidth="1"/>
+    <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
+    <col min="7" max="8" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
@@ -3281,20 +3304,20 @@
       <c r="J1" s="51"/>
       <c r="K1" s="51"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="49"/>
       <c r="B2" s="49"/>
       <c r="C2" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
@@ -3302,18 +3325,18 @@
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="1"/>
@@ -3323,19 +3346,19 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="16.5" customHeight="1">
+    <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -3344,12 +3367,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="16.5" customHeight="1">
+    <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -3357,7 +3380,7 @@
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
       <c r="F5" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3365,9 +3388,9 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3418,59 +3441,59 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="49.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="50" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="35"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>